<commit_message>
updated on 2018-07-19 09:31:00
</commit_message>
<xml_diff>
--- a/PBPS_list.xlsx
+++ b/PBPS_list.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/serdarbalciold/RepTemplates/JournalWatchPBPath/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB9C4B1-F148-C54B-8860-95DEE02C1836}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09EBFB84-A250-E84D-B618-F93FB5926064}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="120" windowWidth="25600" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PBPS list" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -2407,14 +2407,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <color rgb="FF999999"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF999999"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="35">
@@ -2901,7 +2902,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2953,7 +2954,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3181,8 +3182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3240,7 +3241,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -3250,7 +3251,7 @@
       <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="11" t="s">
         <v>729</v>
       </c>
       <c r="F2" s="5" t="s">
@@ -3288,13 +3289,13 @@
       <c r="C3" s="5" t="s">
         <v>597</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>735</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>736</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>734</v>
       </c>
       <c r="H3" s="5" t="s">

</xml_diff>